<commit_message>
ventanas Alquiler 90% listo
</commit_message>
<xml_diff>
--- a/ProyectoFinal/Datos.xlsx
+++ b/ProyectoFinal/Datos.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\NetBeansProjects\GITHUB\proyecto_final_Estructura_de_datos_2022\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3451A22D-F90D-48AE-B17F-0EDB42C9A609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C751C1-D259-4986-A395-5365B18721D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{97392C37-2B9F-4F91-B69C-305730628299}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="745" activeTab="3" xr2:uid="{97392C37-2B9F-4F91-B69C-305730628299}"/>
   </bookViews>
   <sheets>
     <sheet name="vehiculos" sheetId="1" r:id="rId1"/>
     <sheet name="Clientes" sheetId="2" r:id="rId2"/>
     <sheet name="Solicitudes" sheetId="3" r:id="rId3"/>
+    <sheet name="Alquiler" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="48">
   <si>
     <t>Toyota</t>
   </si>
@@ -176,6 +177,9 @@
   </si>
   <si>
     <t>01-12-2022</t>
+  </si>
+  <si>
+    <t>05-12-2022</t>
   </si>
 </sst>
 </file>
@@ -540,7 +544,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +889,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E622A8-5F90-485E-96F1-F7A534C98303}">
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,4 +1074,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAAE86E-3BC4-46CD-AE0F-D2AF4BAF5677}">
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>2022121</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1">
+        <v>506060</v>
+      </c>
+      <c r="D1">
+        <v>22222222</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1">
+        <v>150000</v>
+      </c>
+      <c r="H1">
+        <v>2</v>
+      </c>
+      <c r="I1">
+        <f>300000</f>
+        <v>300000</v>
+      </c>
+      <c r="J1">
+        <v>78000</v>
+      </c>
+      <c r="K1">
+        <v>678000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>